<commit_message>
update to FCA spreadsheet, reomved temp grouping terms from spreadsheets
</commit_message>
<xml_diff>
--- a/cell_type_reports/adult_nephrocytes.xlsx
+++ b/cell_type_reports/adult_nephrocytes.xlsx
@@ -1,37 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cp390/git/drosophila-anatomy-developmental-ontology/cell_type_reports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B2B183-AD4D-7249-A820-0B446ECD0254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="29940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+  <si>
+    <t>FBbt_ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Synonyms</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Review_notes</t>
+  </si>
+  <si>
+    <t>Suggested_markers</t>
+  </si>
+  <si>
+    <t>Abundance</t>
+  </si>
+  <si>
+    <t>adult garland cell</t>
+  </si>
+  <si>
+    <t>nephrocyte</t>
+  </si>
+  <si>
+    <t>Large binucleate garland cell of the adult.</t>
+  </si>
+  <si>
+    <t>Rizki, 1978, Ashburner, Wright, 1978-1980 b: 397--452 (flybase.org/reports/FBrf0031012)</t>
+  </si>
+  <si>
+    <t>adult pericardial cell</t>
+  </si>
+  <si>
+    <t>nephrocyte; Nph; PCl</t>
+  </si>
+  <si>
+    <t>A discrete, large, ovoid cell attached to the dorsal diaphragm in the abdomen and near the anterior end of the ventriculus in the thorax. Some of these cells are binucleate.</t>
+  </si>
+  <si>
+    <t>Miller, 1950, Demerec, 1950: 420--534 (flybase.org/reports/FBrf0007735)</t>
+  </si>
+  <si>
+    <t>adult thoracic pericardial cell</t>
+  </si>
+  <si>
+    <t>Pericardial cell of the adult thorax. These cells are binucleate. There are about 10 on each side, anterior and lateral to the cardia, associated with the lower wall of the trachea leading to the fist spiracle and with the adult salivary gland suspensor muscle (FBbt:00003542).</t>
+  </si>
+  <si>
+    <t>adult abdominal pericardial cell</t>
+  </si>
+  <si>
+    <t>Pcl</t>
+  </si>
+  <si>
+    <t>Pericardial cell of the adult abdomen. These are serially arranges in a row of 20-25 on each side of the hear from the first to the 6th segment.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +129,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,207 +453,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>FBbt_ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Synonyms</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Definition</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>References</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Review_notes</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Suggested_markers</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Abundance</t>
-        </is>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2">
-        <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00048475","FBbt:00048475")</f>
-        <v/>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>adult nephrocyte</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00003183","FBbt:00003183")</f>
+        <v>FBbt:00003183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3">
-        <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00003183","FBbt:00003183")</f>
-        <v/>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>adult garland cell</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>nephrocyte</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Large binucleate garland cell of the adult.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Rizki, 1978, Ashburner, Wright, 1978-1980 b: 397--452 (flybase.org/reports/FBrf0031012)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00003184","FBbt:00003184")</f>
+        <v>FBbt:00003184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="A4">
-        <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00003184","FBbt:00003184")</f>
-        <v/>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>adult pericardial cell</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>nephrocyte; Nph; PCl</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>A discrete, large, ovoid cell attached to the dorsal diaphragm in the abdomen and near the anterior end of the ventriculus in the thorax. Some of these cells are binucleate.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Miller, 1950, Demerec, 1950: 420--534 (flybase.org/reports/FBrf0007735)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00013184","FBbt:00013184")</f>
+        <v>FBbt:00013184</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5">
-      <c r="A5">
-        <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00013184","FBbt:00013184")</f>
-        <v/>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>adult thoracic pericardial cell</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>nephrocyte</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Pericardial cell of the adult thorax. These cells are binucleate. There are about 10 on each side, anterior and lateral to the cardia, associated with the lower wall of the trachea leading to the fist spiracle and with the adult salivary gland suspensor muscle (FBbt:00003542).</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Miller, 1950, Demerec, 1950: 420--534 (flybase.org/reports/FBrf0007735)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
         <f>HYPERLINK("https://www.ebi.ac.uk/ols/ontologies/fbbt/terms?iri=http://purl.obolibrary.org/obo/FBbt_00013185","FBbt:00013185")</f>
-        <v/>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>adult abdominal pericardial cell</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Pcl</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Pericardial cell of the adult abdomen. These are serially arranges in a row of 20-25 on each side of the hear from the first to the 6th segment.</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Miller, 1950, Demerec, 1950: 420--534 (flybase.org/reports/FBrf0007735)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+        <v>FBbt:00013185</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>